<commit_message>
Non-i.i.d. finally working as intended!!!
</commit_message>
<xml_diff>
--- a/fedml/src/main/java/nl/tudelft/trustchain/fedml/ai/gar/ProBristleTest new.xlsx
+++ b/fedml/src/main/java/nl/tudelft/trustchain/fedml/ai/gar/ProBristleTest new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jverb\StudioProjects\trustchain-superapp\fedml\src\main\java\nl\tudelft\trustchain\fedml\ai\gar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C080D4B9-42D8-498D-9B7C-32990AA2C54C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E253F-8931-4286-9B67-8441B2902ABA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{844211C3-7185-423C-9B06-879ED161A981}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
   <si>
     <t>own loss</t>
   </si>
@@ -416,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E1C72C-1D05-4355-8DCC-C2D9B80FA9B3}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1010,7 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>0.9</v>
@@ -1024,7 +1023,7 @@
       </c>
       <c r="F26">
         <f>SUM(B26:D26)</f>
-        <v>2.5</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1032,20 +1031,20 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0.9</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E28" t="s">
         <v>3</v>
       </c>
       <c r="F28">
         <f>SUM(B28:D28)</f>
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1062,45 +1061,21 @@
       </c>
       <c r="D29">
         <f>ABS(D28-D$26) * 10</f>
-        <v>0</v>
+        <v>1.9999999999999996</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B30">
-        <f>MAX(-100, IF(B28&gt;B$26, POWER(B29, 3 + B26), -POWER(B29, 4+B26)))</f>
         <v>0</v>
       </c>
       <c r="C30">
-        <f>MAX(-100, IF(C28&gt;C$26, POWER(C29, 3 + C26), -POWER(C29, 4+C26)))</f>
         <v>0</v>
       </c>
       <c r="D30">
-        <f>MAX(-100, IF(D28&gt;D$26, POWER(D29, 3 + D26), -POWER(D29, 4+D26)))</f>
-        <v>0</v>
-      </c>
-      <c r="E30" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30">
-        <f>MAX(-1000, SUM(B30:D30))</f>
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30">
-        <f xml:space="preserve"> MAX(0, AVERAGE(B28:D28) - _xlfn.STDEV.P(B28:D28) * 2)</f>
-        <v>0.49339869909381451</v>
-      </c>
-      <c r="J30" t="s">
-        <v>2</v>
-      </c>
-      <c r="K30">
-        <f>MAX((1/(1+EXP(-F30/100)))*10-4, 0) * I30</f>
-        <v>0.49339869909381451</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1108,260 +1083,298 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <f>IF(B29&gt;B$26, POWER(B30, 3 + B27), -POWER(B30, 4+B27))</f>
+        <f t="shared" ref="B31:C31" si="8">MAX(-100, IF(B28&gt;B$26, POWER(B29, 3 + B26), -POWER(B29, 4+B26)*(1+B30)))</f>
         <v>0</v>
       </c>
       <c r="C31">
-        <f>MAX(-100, IF(C28&gt;C$26, POWER(C29, 3 + C26), -POWER(C29, 4+C26)))</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="D31">
-        <f>MAX(-100, IF(D29&gt;D$26, POWER(D30, 3 + D27), -POWER(D30, 4+D27)))</f>
-        <v>0</v>
+        <f>MAX(-100, IF(D28&gt;D$26, POWER(D29, 3 + D26), -POWER(D29, 4+D26)*(1+D30)))</f>
+        <v>-31.999999999999964</v>
       </c>
       <c r="E31" t="s">
         <v>3</v>
       </c>
       <c r="F31">
         <f>MAX(-1000, SUM(B31:D31))</f>
-        <v>0</v>
+        <v>-31.999999999999964</v>
       </c>
       <c r="H31" t="s">
         <v>7</v>
       </c>
       <c r="I31">
         <f xml:space="preserve"> MAX(0, AVERAGE(B28:D28) - _xlfn.STDEV.P(B28:D28) * 2)</f>
-        <v>0.49339869909381451</v>
+        <v>0.73670068381445486</v>
       </c>
       <c r="J31" t="s">
         <v>2</v>
       </c>
       <c r="K31">
         <f>MAX((1/(1+EXP(-F31/100)))*10-4, 0) * I31</f>
-        <v>0.49339869909381451</v>
+        <v>0.15231837580391541</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <f>MIN(1, (B28-0.2)*4)</f>
-        <v>1</v>
+        <f t="shared" ref="B32:C32" si="9">MAX(-100, IF(B28&gt;B$26, POWER(B29, 3 + B26), -POWER(B29, 4+B26)*(1+B30)))</f>
+        <v>0</v>
       </c>
       <c r="C32">
-        <f>MIN(1, (C28-0.2)*4)</f>
-        <v>1</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="D32">
-        <f>MIN(1, (D28-0.2)*4)</f>
-        <v>1</v>
+        <f>MAX(-100, IF(D28&gt;D$26, POWER(D29, 3 + D26), -POWER(D29, 4+D26)*(1+D30)))</f>
+        <v>-31.999999999999964</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f>MAX(-1000, SUM(B32:D32))</f>
+        <v>-31.999999999999964</v>
+      </c>
+      <c r="H32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <f xml:space="preserve"> MAX(0, AVERAGE(B28:D28) - _xlfn.STDEV.P(B28:D28) * 2)</f>
+        <v>0.73670068381445486</v>
+      </c>
+      <c r="J32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <f>MAX((1/(1+EXP(-F32/100)))*10-4, 0) * I32</f>
+        <v>0.15231837580391541</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <f>MIN(1, (B28-0.2)*4)</f>
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f>MIN(1, (C28-0.2)*4)</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>MIN(1, (D28-0.2)*4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>8</v>
       </c>
-      <c r="B33">
-        <f>MAX((1/(1+EXP(-B30/100)))*10-4, 0) * B32</f>
-        <v>1</v>
-      </c>
-      <c r="C33">
-        <f>MAX((1/(1+EXP(-C30/100)))*10-4, 0) * C32</f>
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <f>MAX((1/(1+EXP(-D30/100)))*10-4, 0) * D32</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>0.3</v>
-      </c>
-      <c r="C35">
-        <v>0.3</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
+      <c r="B34">
+        <f>MAX((1/(1+EXP(-B31/100)))*10-4, 0) * B33</f>
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <f>MAX((1/(1+EXP(-C31/100)))*10-4, 0) * C33</f>
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <f>MAX((1/(1+EXP(-D31/100)))*10-4, 0) * D33</f>
+        <v>0.2067574785125057</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B36">
-        <f>ABS(B35-B$26) * 10</f>
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="C36">
-        <f>ABS(C35-C$26) * 10</f>
-        <v>6.0000000000000009</v>
+        <v>0.3</v>
       </c>
       <c r="D36">
-        <f>ABS(D35-D$26) * 10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37">
-        <f>MAX(0, 2*(B$26-B$28))</f>
-        <v>0</v>
+        <f>ABS(B36-B$26) * 10</f>
+        <v>7</v>
       </c>
       <c r="C37">
-        <f>MAX(0, 2*(C$26-C$28))</f>
-        <v>0</v>
+        <f>ABS(C36-C$26) * 10</f>
+        <v>6.0000000000000009</v>
       </c>
       <c r="D37">
-        <f>MAX(0, 2*(D$26-D$28))</f>
+        <f>ABS(D36-D$26) * 10</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B38">
-        <f>MAX(-100, IF(B35&gt;B$26, POWER(B36, 3 + B26), -POWER(B36, 4+B26)*(1+B37)))</f>
-        <v>-100</v>
+        <f>MAX(0, 2*(B$26-B$28))</f>
+        <v>0</v>
       </c>
       <c r="C38">
-        <f>MAX(-100, IF(C35&gt;C$26, POWER(C36, 3 + C26), -POWER(C36, 4+C26)*(1+C37)))</f>
-        <v>-100</v>
+        <f>MAX(0, 2*(C$26-C$28))</f>
+        <v>0</v>
       </c>
       <c r="D38">
-        <f>MAX(-100, IF(D35&gt;D$26, POWER(D36, 3 + D26), -POWER(D36, 4+D26)*(1+D37)))</f>
-        <v>0</v>
-      </c>
-      <c r="E38" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38">
-        <f>MAX(-1000, SUM(B38:D38))</f>
-        <v>-200</v>
-      </c>
-      <c r="H38" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38">
-        <f xml:space="preserve"> MAX(0, AVERAGE(B35:K35) - _xlfn.STDEV.P(B35:K35) * 2)</f>
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
-        <v>2</v>
-      </c>
-      <c r="K38">
-        <f>MAX((1/(1+EXP(-F38/100)))*10-4, 0) * I38</f>
-        <v>0</v>
+        <f>MAX(0, 2*(D$26-D$28))</f>
+        <v>0.39999999999999991</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <f>MAX(-100, IF(B36&gt;B$26, POWER(B37, 3 + B26), -POWER(B37, 4+B26)*(1+B38)))</f>
+        <v>-100</v>
+      </c>
+      <c r="C39">
+        <f>MAX(-100, IF(C36&gt;C$26, POWER(C37, 3 + C26), -POWER(C37, 4+C26)*(1+C38)))</f>
+        <v>-100</v>
+      </c>
+      <c r="D39">
+        <f>MAX(-100, IF(D36&gt;D$26, POWER(D37, 3 + D26), -POWER(D37, 4+D26)*(1+D38)))</f>
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <f>MAX(-1000, SUM(B39:D39))</f>
+        <v>-200</v>
+      </c>
+      <c r="H39" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39">
+        <f xml:space="preserve"> MAX(0, AVERAGE(B36:K36) - _xlfn.STDEV.P(B36:K36) * 2)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>2</v>
+      </c>
+      <c r="K39">
+        <f>MAX((1/(1+EXP(-F39/100)))*10-4, 0) * I39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>8</v>
       </c>
-      <c r="B39">
-        <f>MAX((1/(1+EXP(-B38/100)))*10-4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <f>MAX((1/(1+EXP(-C38/100)))*10-4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <f>MAX((1/(1+EXP(-D38/100)))*10-4, 0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
+      <c r="B40">
+        <f>MAX((1/(1+EXP(-B39/100)))*10-4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f>MAX((1/(1+EXP(-C39/100)))*10-4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <f>MAX((1/(1+EXP(-D39/100)))*10-4, 0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B42">
-        <f>ABS(B41-B$1)*10*IF(B26&gt;=B41, AVERAGE($B26:$K26), 1)</f>
-        <v>3.0000000000000004</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <f>ABS(C41-C$1)*10*IF(C26&gt;=C41, AVERAGE($B26:$K26), 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <f>ABS(D41-D$1)*10*IF(D26&gt;=D41, AVERAGE($B26:$K26), 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <f>ABS(B42-B$1)*10*IF(B26&gt;=B42, AVERAGE($B26:$K26), 1)</f>
+        <v>4.3500000000000005</v>
+      </c>
+      <c r="C43">
+        <f>ABS(C42-C$1)*10*IF(C26&gt;=C42, AVERAGE($B26:$K26), 1)</f>
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <f>ABS(D42-D$1)*10*IF(D26&gt;=D42, AVERAGE($B26:$K26), 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <f>MAX(0, 2*(B$1+B$1-B$3-B$7))</f>
         <v>0</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <f>MAX(0, 2*(C$1+C$1-C$3-C$7))</f>
         <v>0.20000000000000018</v>
       </c>
-      <c r="D43">
+      <c r="D44">
         <f>MAX(0, 2*(D$1+D$1-D$3-D$7))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B44">
-        <f>IF(B41&gt;B$1, POWER(B42, 2+B$1*1.5), -POWER(B42, 3+B$1*1.5)*(1+B43))</f>
-        <v>28.524617330837529</v>
-      </c>
-      <c r="C44">
-        <f>IF(C41&gt;C$1, POWER(C42, 2+C$1*1.5), -POWER(C42, 3+C$1*1.5)*(1+C43))</f>
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <f>IF(D41&gt;D$1, POWER(D42, 2+D$1*1.5), -POWER(D42, 3+D$1*1.5)*(1+D43))</f>
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="B45">
+        <f>IF(B42&gt;B$1, POWER(B43, 2+B$1*1.5), -POWER(B43, 3+B$1*1.5)*(1+B44))</f>
+        <v>88.591536441464001</v>
+      </c>
+      <c r="C45">
+        <f>IF(C42&gt;C$1, POWER(C43, 2+C$1*1.5), -POWER(C43, 3+C$1*1.5)*(1+C44))</f>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f>IF(D42&gt;D$1, POWER(D43, 2+D$1*1.5), -POWER(D43, 3+D$1*1.5)*(1+D44))</f>
+        <v>0</v>
+      </c>
+      <c r="E45" t="s">
         <v>3</v>
       </c>
-      <c r="F44">
-        <f>MAX(-1000, SUM(B44:D44))</f>
-        <v>28.524617330837529</v>
-      </c>
-      <c r="H44" t="s">
+      <c r="F45">
+        <f>MAX(-1000, SUM(B45:D45))</f>
+        <v>88.591536441464001</v>
+      </c>
+      <c r="H45" t="s">
         <v>7</v>
       </c>
-      <c r="I44">
-        <f xml:space="preserve"> MAX(0, AVERAGE(B41:K41) - _xlfn.STDEV.P(B41:K41) * 2)</f>
-        <v>1</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="I45">
+        <f xml:space="preserve"> MAX(0, AVERAGE(B42:K42) - _xlfn.STDEV.P(B42:K42) * 2)</f>
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
         <v>2</v>
       </c>
-      <c r="K44">
-        <f>MAX((1/(1+EXP(-F44/100)))*10-4, 0) * I44</f>
-        <v>1.7083192118175328</v>
+      <c r="K45">
+        <f>MAX((1/(1+EXP(-F45/100)))*10-4, 0) * I45</f>
+        <v>3.0804652851105851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>